<commit_message>
add new feature hot daily market data download to csv
</commit_message>
<xml_diff>
--- a/Trading_BackTest_on_VNPY/examples/VNPY2_BILLY/Batch_CTABacktesting/ctaStrategy.xlsx
+++ b/Trading_BackTest_on_VNPY/examples/VNPY2_BILLY/Batch_CTABacktesting/ctaStrategy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sap-my.sharepoint.com/personal/billy_zhang02_sap_com/Documents/Desktop/Downloads/Trading_BackTest_on_VNPY/examples/VNPY2_BILLY/Batch_CTABacktesting/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="36" documentId="13_ncr:1_{162AEA55-4988-433C-B859-1C2FB76CB11C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DDCEE8A4-0F86-420C-AD9D-95EBD8D271B4}"/>
+  <xr:revisionPtr revIDLastSave="39" documentId="13_ncr:1_{162AEA55-4988-433C-B859-1C2FB76CB11C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8EC02E69-6DFC-4004-AF35-503677708661}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2955" yWindow="2055" windowWidth="17250" windowHeight="10095" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="810" uniqueCount="274">
   <si>
     <t>class_name</t>
   </si>
@@ -47,316 +47,814 @@
     <t>BarEMaTrendStrategy</t>
   </si>
   <si>
-    <t>ag9999.SHFE</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 3, 'OPEN_RATIO': 0.5, 'MARK_DOWN': 3, 'MARK_UP': 3}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 7, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 3, 'OPEN_RATIO': 0.5, 'MARK_DOWN': 3, 'MARK_UP': 3}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 3, 'OPEN_RATIO': 0.5, 'MARK_DOWN': 6, 'MARK_UP': 3}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 5, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 3, 'OPEN_RATIO': 0.5, 'MARK_DOWN': 3, 'MARK_UP': 3}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 5, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 3, 'OPEN_RATIO': 0.5, 'MARK_DOWN': 6, 'MARK_UP': 3}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 3, 'OPEN_RATIO': 1.0, 'MARK_DOWN': 3, 'MARK_UP': 3}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 3, 'OPEN_RATIO': 1.0, 'MARK_DOWN': 6, 'MARK_UP': 3}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 7, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 5, 'OPEN_RATIO': 0.5, 'MARK_DOWN': 6, 'MARK_UP': 3}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 7, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 3, 'OPEN_RATIO': 0.5, 'MARK_DOWN': 3, 'MARK_UP': 3}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 5, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 3, 'OPEN_RATIO': 0.5, 'MARK_DOWN': 3, 'MARK_UP': 3}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 7, 'SLOW_LENGTH': 40, 'CUT_LENGTH': 5, 'OPEN_RATIO': 0.5, 'MARK_DOWN': 6, 'MARK_UP': 3}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 5, 'SLOW_LENGTH': 40, 'CUT_LENGTH': 3, 'OPEN_RATIO': 0.5, 'MARK_DOWN': 3, 'MARK_UP': 3}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 5, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 3, 'OPEN_RATIO': 1.0, 'MARK_DOWN': 3, 'MARK_UP': 3}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 3, 'OPEN_RATIO': 1.5, 'MARK_DOWN': 6, 'MARK_UP': 3}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 5, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 3, 'OPEN_RATIO': 1.0, 'MARK_DOWN': 3, 'MARK_UP': 3}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 7, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 3, 'OPEN_RATIO': 1.0, 'MARK_DOWN': 3, 'MARK_UP': 3}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 7, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 3, 'OPEN_RATIO': 0.5, 'MARK_DOWN': 6, 'MARK_UP': 3}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 7, 'SLOW_LENGTH': 50, 'CUT_LENGTH': 3, 'OPEN_RATIO': 0.5, 'MARK_DOWN': 6, 'MARK_UP': 3}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 5, 'SLOW_LENGTH': 50, 'CUT_LENGTH': 3, 'OPEN_RATIO': 0.5, 'MARK_DOWN': 3, 'MARK_UP': 3}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 7, 'SLOW_LENGTH': 50, 'CUT_LENGTH': 3, 'OPEN_RATIO': 0.5, 'MARK_DOWN': 3, 'MARK_UP': 3}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 5, 'SLOW_LENGTH': 40, 'CUT_LENGTH': 3, 'OPEN_RATIO': 0.5, 'MARK_DOWN': 6, 'MARK_UP': 3}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 7, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 5, 'OPEN_RATIO': 0.5, 'MARK_DOWN': 6, 'MARK_UP': 3}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 5, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 3, 'OPEN_RATIO': 1.0, 'MARK_DOWN': 6, 'MARK_UP': 3}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 7, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 3, 'OPEN_RATIO': 1.0, 'MARK_DOWN': 6, 'MARK_UP': 3}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 7, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 5, 'OPEN_RATIO': 0.5, 'MARK_DOWN': 9, 'MARK_UP': 6}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 7, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 5, 'OPEN_RATIO': 0.5, 'MARK_DOWN': 3, 'MARK_UP': 3}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 5, 'SLOW_LENGTH': 50, 'CUT_LENGTH': 5, 'OPEN_RATIO': 1.0, 'MARK_DOWN': 6, 'MARK_UP': 3}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 3, 'OPEN_RATIO': 1.5, 'MARK_DOWN': 3, 'MARK_UP': 3}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 5, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 3, 'OPEN_RATIO': 0.5, 'MARK_DOWN': 6, 'MARK_UP': 3}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 7, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 3, 'OPEN_RATIO': 0.5, 'MARK_DOWN': 6, 'MARK_UP': 3}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 7, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 3, 'OPEN_RATIO': 1.5, 'MARK_DOWN': 6, 'MARK_UP': 3}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 5, 'SLOW_LENGTH': 40, 'CUT_LENGTH': 3, 'OPEN_RATIO': 1.0, 'MARK_DOWN': 3, 'MARK_UP': 3}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 7, 'SLOW_LENGTH': 40, 'CUT_LENGTH': 3, 'OPEN_RATIO': 0.5, 'MARK_DOWN': 3, 'MARK_UP': 3}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 3, 'OPEN_RATIO': 1.0, 'MARK_DOWN': 3, 'MARK_UP': 3}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 40, 'CUT_LENGTH': 3, 'OPEN_RATIO': 0.5, 'MARK_DOWN': 3, 'MARK_UP': 3}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 40, 'CUT_LENGTH': 3, 'OPEN_RATIO': 1.0, 'MARK_DOWN': 6, 'MARK_UP': 3}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 7, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 5, 'OPEN_RATIO': 0.5, 'MARK_DOWN': 6, 'MARK_UP': 6}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 3, 'OPEN_RATIO': 0.5, 'MARK_DOWN': 6, 'MARK_UP': 3}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 7, 'SLOW_LENGTH': 40, 'CUT_LENGTH': 5, 'OPEN_RATIO': 1.0, 'MARK_DOWN': 6, 'MARK_UP': 3}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 7, 'SLOW_LENGTH': 50, 'CUT_LENGTH': 3, 'OPEN_RATIO': 2.0, 'MARK_DOWN': 6, 'MARK_UP': 3}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 7, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0.5, 'MARK_DOWN': 6, 'MARK_UP': 3}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 3, 'OPEN_RATIO': 0.5, 'MARK_DOWN': 3, 'MARK_UP': 3}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 5, 'SLOW_LENGTH': 40, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0.5, 'MARK_DOWN': 6, 'MARK_UP': 3}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 7, 'SLOW_LENGTH': 50, 'CUT_LENGTH': 3, 'OPEN_RATIO': 1.0, 'MARK_DOWN': 6, 'MARK_UP': 3}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 7, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 5, 'OPEN_RATIO': 0.5, 'MARK_DOWN': 3, 'MARK_UP': 3}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 5, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 5, 'OPEN_RATIO': 1.5, 'MARK_DOWN': 6, 'MARK_UP': 3}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 40, 'CUT_LENGTH': 3, 'OPEN_RATIO': 1.0, 'MARK_DOWN': 3, 'MARK_UP': 3}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 5, 'SLOW_LENGTH': 50, 'CUT_LENGTH': 5, 'OPEN_RATIO': 1.0, 'MARK_DOWN': 3, 'MARK_UP': 3}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 3, 'OPEN_RATIO': 1.0, 'MARK_DOWN': 6, 'MARK_UP': 3}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 5, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 3, 'OPEN_RATIO': 2.0, 'MARK_DOWN': 6, 'MARK_UP': 3}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 7, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 5, 'OPEN_RATIO': 1.0, 'MARK_DOWN': 6, 'MARK_UP': 3}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 5, 'SLOW_LENGTH': 40, 'CUT_LENGTH': 3, 'OPEN_RATIO': 1.0, 'MARK_DOWN': 6, 'MARK_UP': 3}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 7, 'SLOW_LENGTH': 40, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.0, 'MARK_DOWN': 6, 'MARK_UP': 3}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 7, 'SLOW_LENGTH': 50, 'CUT_LENGTH': 3, 'OPEN_RATIO': 2.0, 'MARK_DOWN': 3, 'MARK_UP': 3}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 7, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 5, 'OPEN_RATIO': 0.5, 'MARK_DOWN': 6, 'MARK_UP': 6}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 5, 'SLOW_LENGTH': 40, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0.5, 'MARK_DOWN': 3, 'MARK_UP': 3}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 40, 'CUT_LENGTH': 3, 'OPEN_RATIO': 0.5, 'MARK_DOWN': 6, 'MARK_UP': 3}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 3, 'OPEN_RATIO': 1.5, 'MARK_DOWN': 3, 'MARK_UP': 3}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 7, 'SLOW_LENGTH': 40, 'CUT_LENGTH': 5, 'OPEN_RATIO': 2.0, 'MARK_DOWN': 6, 'MARK_UP': 3}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 7, 'SLOW_LENGTH': 40, 'CUT_LENGTH': 5, 'OPEN_RATIO': 1.0, 'MARK_DOWN': 3, 'MARK_UP': 3}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 5, 'SLOW_LENGTH': 40, 'CUT_LENGTH': 3, 'OPEN_RATIO': 1.5, 'MARK_DOWN': 3, 'MARK_UP': 3}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 7, 'SLOW_LENGTH': 50, 'CUT_LENGTH': 3, 'OPEN_RATIO': 1.0, 'MARK_DOWN': 3, 'MARK_UP': 3}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 5, 'SLOW_LENGTH': 50, 'CUT_LENGTH': 3, 'OPEN_RATIO': 1.5, 'MARK_DOWN': 3, 'MARK_UP': 3}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 5, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 5, 'OPEN_RATIO': 1.0, 'MARK_DOWN': 6, 'MARK_UP': 3}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 7, 'SLOW_LENGTH': 40, 'CUT_LENGTH': 3, 'OPEN_RATIO': 0.5, 'MARK_DOWN': 6, 'MARK_UP': 3}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 5, 'SLOW_LENGTH': 50, 'CUT_LENGTH': 5, 'OPEN_RATIO': 0.5, 'MARK_DOWN': 6, 'MARK_UP': 3}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 5, 'SLOW_LENGTH': 40, 'CUT_LENGTH': 5, 'OPEN_RATIO': 1.5, 'MARK_DOWN': 6, 'MARK_UP': 3}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 5, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 3, 'OPEN_RATIO': 1.5, 'MARK_DOWN': 6, 'MARK_UP': 3}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 5, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 3, 'OPEN_RATIO': 1.5, 'MARK_DOWN': 3, 'MARK_UP': 3}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 5, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 5, 'OPEN_RATIO': 0.5, 'MARK_DOWN': 3, 'MARK_UP': 3}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 7, 'SLOW_LENGTH': 50, 'CUT_LENGTH': 3, 'OPEN_RATIO': 1.0, 'MARK_DOWN': 6, 'MARK_UP': 6}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 7, 'SLOW_LENGTH': 40, 'CUT_LENGTH': 5, 'OPEN_RATIO': 2.0, 'MARK_DOWN': 9, 'MARK_UP': 6}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 5, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0.5, 'MARK_DOWN': 6, 'MARK_UP': 3}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 7, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 5, 'OPEN_RATIO': 1.5, 'MARK_DOWN': 6, 'MARK_UP': 3}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 50, 'CUT_LENGTH': 3, 'OPEN_RATIO': 1.0, 'MARK_DOWN': 3, 'MARK_UP': 3}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 5, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 5, 'OPEN_RATIO': 0.5, 'MARK_DOWN': 6, 'MARK_UP': 3}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 7, 'SLOW_LENGTH': 40, 'CUT_LENGTH': 5, 'OPEN_RATIO': 2.0, 'MARK_DOWN': 6, 'MARK_UP': 6}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 5, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 5, 'OPEN_RATIO': 1.0, 'MARK_DOWN': 3, 'MARK_UP': 3}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 7, 'SLOW_LENGTH': 40, 'CUT_LENGTH': 5, 'OPEN_RATIO': 1.5, 'MARK_DOWN': 9, 'MARK_UP': 6}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 50, 'CUT_LENGTH': 3, 'OPEN_RATIO': 1.5, 'MARK_DOWN': 6, 'MARK_UP': 6}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 3, 'OPEN_RATIO': 2.0, 'MARK_DOWN': 3, 'MARK_UP': 3}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 5, 'SLOW_LENGTH': 40, 'CUT_LENGTH': 5, 'OPEN_RATIO': 1.0, 'MARK_DOWN': 6, 'MARK_UP': 3}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 7, 'SLOW_LENGTH': 50, 'CUT_LENGTH': 5, 'OPEN_RATIO': 2.0, 'MARK_DOWN': 9, 'MARK_UP': 6}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 5, 'OPEN_RATIO': 0.5, 'MARK_DOWN': 6, 'MARK_UP': 3}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 7, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 3, 'OPEN_RATIO': 0.5, 'MARK_DOWN': 3, 'MARK_UP': 6}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 7, 'SLOW_LENGTH': 50, 'CUT_LENGTH': 5, 'OPEN_RATIO': 2.0, 'MARK_DOWN': 6, 'MARK_UP': 3}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 7, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 3, 'OPEN_RATIO': 1.0, 'MARK_DOWN': 6, 'MARK_UP': 6}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 7, 'SLOW_LENGTH': 50, 'CUT_LENGTH': 3, 'OPEN_RATIO': 1.5, 'MARK_DOWN': 3, 'MARK_UP': 3}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 7, 'SLOW_LENGTH': 50, 'CUT_LENGTH': 5, 'OPEN_RATIO': 1.0, 'MARK_DOWN': 6, 'MARK_UP': 3}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 5, 'SLOW_LENGTH': 50, 'CUT_LENGTH': 3, 'OPEN_RATIO': 1.0, 'MARK_DOWN': 3, 'MARK_UP': 3}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 7, 'SLOW_LENGTH': 50, 'CUT_LENGTH': 5, 'OPEN_RATIO': 1.0, 'MARK_DOWN': 3, 'MARK_UP': 3}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 7, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 3, 'OPEN_RATIO': 2.0, 'MARK_DOWN': 6, 'MARK_UP': 3}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 7, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 5, 'OPEN_RATIO': 0.5, 'MARK_DOWN': 6, 'MARK_UP': 9}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 7, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 5, 'OPEN_RATIO': 0.5, 'MARK_DOWN': 3, 'MARK_UP': 6}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 50, 'CUT_LENGTH': 3, 'OPEN_RATIO': 1.5, 'MARK_DOWN': 3, 'MARK_UP': 3}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 7, 'SLOW_LENGTH': 40, 'CUT_LENGTH': 5, 'OPEN_RATIO': 1.5, 'MARK_DOWN': 6, 'MARK_UP': 6}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 7, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 3, 'OPEN_RATIO': 1.5, 'MARK_DOWN': 3, 'MARK_UP': 3}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 5, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 5, 'OPEN_RATIO': 1.5, 'MARK_DOWN': 6, 'MARK_UP': 6}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 50, 'CUT_LENGTH': 3, 'OPEN_RATIO': 2.0, 'MARK_DOWN': 6, 'MARK_UP': 3}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 5, 'SLOW_LENGTH': 50, 'CUT_LENGTH': 3, 'OPEN_RATIO': 1.5, 'MARK_DOWN': 6, 'MARK_UP': 3}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 5, 'SLOW_LENGTH': 50, 'CUT_LENGTH': 3, 'OPEN_RATIO': 0.5, 'MARK_DOWN': 6, 'MARK_UP': 3}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 50, 'CUT_LENGTH': 3, 'OPEN_RATIO': 0.5, 'MARK_DOWN': 3, 'MARK_UP': 3}</t>
-  </si>
-  <si>
-    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 1, 'CLOSE_WINDOWS': 16, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 40, 'CUT_LENGTH': 3, 'OPEN_RATIO': 1.5, 'MARK_DOWN': 3, 'MARK_UP': 3}</t>
+    <t>fu9999.SHFE</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 2.0, 'MARK_DOWN': 8, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.5, 'MARK_DOWN': 8, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 10, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.0, 'MARK_DOWN': 8, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.0, 'MARK_DOWN': 8, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 10, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0, 'MARK_DOWN': 8, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0.5, 'MARK_DOWN': 8, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 10, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 2.0, 'MARK_DOWN': 8, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 10, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.5, 'MARK_DOWN': 8, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 5, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.0, 'MARK_DOWN': 8, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0, 'MARK_DOWN': 8, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 5, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0, 'MARK_DOWN': 8, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 10, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0.5, 'MARK_DOWN': 8, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 5, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.5, 'MARK_DOWN': 8, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 5, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 2.0, 'MARK_DOWN': 8, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 5, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0.5, 'MARK_DOWN': 8, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0, 'MARK_DOWN': 8, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 2.5, 'MARK_DOWN': 8, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 10, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0, 'MARK_DOWN': 8, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 5, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 2.5, 'MARK_DOWN': 8, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 10, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 2.5, 'MARK_DOWN': 8, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 2.0, 'MARK_DOWN': 8, 'MARK_UP': 6}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.0, 'MARK_DOWN': 8, 'MARK_UP': 6}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 10, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0, 'MARK_DOWN': 8, 'MARK_UP': 4}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 10, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0, 'MARK_DOWN': 8, 'MARK_UP': 6}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.5, 'MARK_DOWN': 8, 'MARK_UP': 6}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0.5, 'MARK_DOWN': 8, 'MARK_UP': 4}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0.5, 'MARK_DOWN': 8, 'MARK_UP': 6}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 2.0, 'MARK_DOWN': 8, 'MARK_UP': 4}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 10, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.0, 'MARK_DOWN': 8, 'MARK_UP': 6}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.0, 'MARK_DOWN': 8, 'MARK_UP': 4}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 10, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 2.0, 'MARK_DOWN': 8, 'MARK_UP': 6}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 10, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.5, 'MARK_DOWN': 8, 'MARK_UP': 6}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0, 'MARK_DOWN': 8, 'MARK_UP': 4}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0, 'MARK_DOWN': 8, 'MARK_UP': 6}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 10, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0.5, 'MARK_DOWN': 8, 'MARK_UP': 4}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 10, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0.5, 'MARK_DOWN': 8, 'MARK_UP': 6}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.5, 'MARK_DOWN': 8, 'MARK_UP': 4}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 5, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 2.0, 'MARK_DOWN': 6, 'MARK_UP': 6}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 5, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 2.0, 'MARK_DOWN': 6, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 5, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 2.0, 'MARK_DOWN': 8, 'MARK_UP': 6}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 2.0, 'MARK_DOWN': 6, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0, 'MARK_DOWN': 6, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 2.0, 'MARK_DOWN': 6, 'MARK_UP': 6}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0, 'MARK_DOWN': 6, 'MARK_UP': 4}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0, 'MARK_DOWN': 6, 'MARK_UP': 6}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.0, 'MARK_DOWN': 6, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 10, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.0, 'MARK_DOWN': 8, 'MARK_UP': 4}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.0, 'MARK_DOWN': 6, 'MARK_UP': 6}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 5, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.0, 'MARK_DOWN': 6, 'MARK_UP': 6}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 5, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.0, 'MARK_DOWN': 6, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 5, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.0, 'MARK_DOWN': 8, 'MARK_UP': 6}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 10, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 2.0, 'MARK_DOWN': 8, 'MARK_UP': 4}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0.5, 'MARK_DOWN': 6, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 7, 'OPEN_RATIO': 2.0, 'MARK_DOWN': 6, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.5, 'MARK_DOWN': 6, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 5, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.5, 'MARK_DOWN': 6, 'MARK_UP': 6}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 5, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.5, 'MARK_DOWN': 6, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 5, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.5, 'MARK_DOWN': 8, 'MARK_UP': 6}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0.5, 'MARK_DOWN': 6, 'MARK_UP': 4}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0.5, 'MARK_DOWN': 6, 'MARK_UP': 6}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 10, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.0, 'MARK_DOWN': 6, 'MARK_UP': 6}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 10, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.0, 'MARK_DOWN': 6, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 10, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 7, 'OPEN_RATIO': 2.0, 'MARK_DOWN': 6, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.5, 'MARK_DOWN': 6, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 10, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.5, 'MARK_DOWN': 8, 'MARK_UP': 4}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 10, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 2.0, 'MARK_DOWN': 6, 'MARK_UP': 6}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 10, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 2.0, 'MARK_DOWN': 6, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 10, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.5, 'MARK_DOWN': 6, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.5, 'MARK_DOWN': 6, 'MARK_UP': 6}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.0, 'MARK_DOWN': 4, 'MARK_UP': 6}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.0, 'MARK_DOWN': 4, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 10, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0, 'MARK_DOWN': 6, 'MARK_UP': 4}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 10, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0, 'MARK_DOWN': 6, 'MARK_UP': 6}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 10, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0, 'MARK_DOWN': 6, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0.5, 'MARK_DOWN': 4, 'MARK_UP': 6}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0.5, 'MARK_DOWN': 4, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 10, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.5, 'MARK_DOWN': 6, 'MARK_UP': 6}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 10, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.5, 'MARK_DOWN': 6, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0, 'MARK_DOWN': 4, 'MARK_UP': 6}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 10, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 7, 'OPEN_RATIO': 2.0, 'MARK_DOWN': 8, 'MARK_UP': 4}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 10, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 7, 'OPEN_RATIO': 2.0, 'MARK_DOWN': 8, 'MARK_UP': 6}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 10, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 7, 'OPEN_RATIO': 2.0, 'MARK_DOWN': 8, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 5, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0, 'MARK_DOWN': 6, 'MARK_UP': 4}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 5, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0, 'MARK_DOWN': 6, 'MARK_UP': 6}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 5, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0, 'MARK_DOWN': 6, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 5, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0, 'MARK_DOWN': 8, 'MARK_UP': 4}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 5, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0, 'MARK_DOWN': 8, 'MARK_UP': 6}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0, 'MARK_DOWN': 4, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 5, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 2.0, 'MARK_DOWN': 8, 'MARK_UP': 4}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 10, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.5, 'MARK_DOWN': 8, 'MARK_UP': 4}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 10, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.5, 'MARK_DOWN': 8, 'MARK_UP': 6}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 10, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.5, 'MARK_DOWN': 8, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 7, 'OPEN_RATIO': 2.0, 'MARK_DOWN': 6, 'MARK_UP': 4}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 2.5, 'MARK_DOWN': 8, 'MARK_UP': 6}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.5, 'MARK_DOWN': 6, 'MARK_UP': 4}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 5, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 2.0, 'MARK_DOWN': 6, 'MARK_UP': 4}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 2.0, 'MARK_DOWN': 6, 'MARK_UP': 4}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 5, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0.5, 'MARK_DOWN': 6, 'MARK_UP': 4}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 5, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0.5, 'MARK_DOWN': 6, 'MARK_UP': 6}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 5, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0.5, 'MARK_DOWN': 6, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 5, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0.5, 'MARK_DOWN': 8, 'MARK_UP': 4}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 5, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0.5, 'MARK_DOWN': 8, 'MARK_UP': 6}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 7, 'OPEN_RATIO': 2.0, 'MARK_DOWN': 8, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 10, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 7, 'SLOW_LENGTH': 40, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.5, 'MARK_DOWN': 4, 'MARK_UP': 4}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 10, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0.5, 'MARK_DOWN': 6, 'MARK_UP': 4}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 10, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0.5, 'MARK_DOWN': 6, 'MARK_UP': 6}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 10, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0.5, 'MARK_DOWN': 6, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.5, 'MARK_DOWN': 8, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 7, 'OPEN_RATIO': 2.0, 'MARK_DOWN': 8, 'MARK_UP': 4}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 7, 'OPEN_RATIO': 2.0, 'MARK_DOWN': 8, 'MARK_UP': 6}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.0, 'MARK_DOWN': 6, 'MARK_UP': 4}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 5, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.0, 'MARK_DOWN': 8, 'MARK_UP': 4}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.5, 'MARK_DOWN': 8, 'MARK_UP': 4}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.5, 'MARK_DOWN': 8, 'MARK_UP': 6}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 7, 'OPEN_RATIO': 2.0, 'MARK_DOWN': 4, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 5, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.0, 'MARK_DOWN': 6, 'MARK_UP': 4}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 10, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 7, 'OPEN_RATIO': 2.0, 'MARK_DOWN': 6, 'MARK_UP': 4}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 10, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 7, 'OPEN_RATIO': 2.0, 'MARK_DOWN': 6, 'MARK_UP': 6}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 5, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.5, 'MARK_DOWN': 8, 'MARK_UP': 4}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 10, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.5, 'MARK_DOWN': 6, 'MARK_UP': 4}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 10, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.5, 'MARK_DOWN': 6, 'MARK_UP': 6}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.5, 'MARK_DOWN': 4, 'MARK_UP': 6}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.5, 'MARK_DOWN': 4, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 10, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.0, 'MARK_DOWN': 4, 'MARK_UP': 6}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 10, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.0, 'MARK_DOWN': 4, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 7, 'OPEN_RATIO': 2.0, 'MARK_DOWN': 6, 'MARK_UP': 6}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 2.0, 'MARK_DOWN': 4, 'MARK_UP': 6}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 2.0, 'MARK_DOWN': 4, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.5, 'MARK_DOWN': 6, 'MARK_UP': 6}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 5, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 2.5, 'MARK_DOWN': 6, 'MARK_UP': 6}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 5, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 2.5, 'MARK_DOWN': 6, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 5, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 2.5, 'MARK_DOWN': 8, 'MARK_UP': 6}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 5, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.5, 'MARK_DOWN': 6, 'MARK_UP': 4}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 10, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.0, 'MARK_DOWN': 6, 'MARK_UP': 4}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.5, 'MARK_DOWN': 6, 'MARK_UP': 4}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0.5, 'MARK_DOWN': 4, 'MARK_UP': 4}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 10, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 2.0, 'MARK_DOWN': 6, 'MARK_UP': 4}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.5, 'MARK_DOWN': 4, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 2.5, 'MARK_DOWN': 8, 'MARK_UP': 4}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0, 'MARK_DOWN': 4, 'MARK_UP': 4}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 10, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0.5, 'MARK_DOWN': 8, 'MARK_UP': 4}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 10, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0.5, 'MARK_DOWN': 8, 'MARK_UP': 6}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 10, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0.5, 'MARK_DOWN': 8, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 50, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0, 'MARK_DOWN': 8, 'MARK_UP': 6}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 50, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0, 'MARK_DOWN': 8, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 10, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0.5, 'MARK_DOWN': 4, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 10, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 7, 'SLOW_LENGTH': 40, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.5, 'MARK_DOWN': 4, 'MARK_UP': 6}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 10, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0, 'MARK_DOWN': 4, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 10, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 7, 'OPEN_RATIO': 2.5, 'MARK_DOWN': 6, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 10, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.5, 'MARK_DOWN': 6, 'MARK_UP': 4}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 10, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0.5, 'MARK_DOWN': 4, 'MARK_UP': 6}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 10, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0, 'MARK_DOWN': 4, 'MARK_UP': 6}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 10, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 7, 'SLOW_LENGTH': 40, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.5, 'MARK_DOWN': 8, 'MARK_UP': 6}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 10, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.5, 'MARK_DOWN': 4, 'MARK_UP': 6}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 10, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.5, 'MARK_DOWN': 4, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 10, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 7, 'OPEN_RATIO': 2.0, 'MARK_DOWN': 4, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 10, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 7, 'SLOW_LENGTH': 40, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.5, 'MARK_DOWN': 8, 'MARK_UP': 4}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 10, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 7, 'SLOW_LENGTH': 40, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.0, 'MARK_DOWN': 4, 'MARK_UP': 4}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0, 'MARK_DOWN': 8, 'MARK_UP': 4}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0, 'MARK_DOWN': 8, 'MARK_UP': 6}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 10, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0, 'MARK_DOWN': 8, 'MARK_UP': 4}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 10, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0, 'MARK_DOWN': 8, 'MARK_UP': 6}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 10, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 7, 'SLOW_LENGTH': 40, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.5, 'MARK_DOWN': 4, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 2.5, 'MARK_DOWN': 6, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 50, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0, 'MARK_DOWN': 8, 'MARK_UP': 4}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 5, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 2.0, 'MARK_DOWN': 4, 'MARK_UP': 6}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 5, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 2.0, 'MARK_DOWN': 4, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 2.5, 'MARK_DOWN': 6, 'MARK_UP': 6}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 5, 'CLOSE_WINDOWS': 10, 'QUICK_LENGTH': 7, 'SLOW_LENGTH': 50, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0, 'MARK_DOWN': 6, 'MARK_UP': 4}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0.5, 'MARK_DOWN': 8, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 10, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 2.5, 'MARK_DOWN': 8, 'MARK_UP': 6}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0.5, 'MARK_DOWN': 6, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0.5, 'MARK_DOWN': 8, 'MARK_UP': 4}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0.5, 'MARK_DOWN': 8, 'MARK_UP': 6}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 50, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0, 'MARK_DOWN': 6, 'MARK_UP': 6}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 10, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.5, 'MARK_DOWN': 4, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 7, 'OPEN_RATIO': 2.5, 'MARK_DOWN': 4, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 7, 'OPEN_RATIO': 2.0, 'MARK_DOWN': 4, 'MARK_UP': 6}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 10, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0.5, 'MARK_DOWN': 6, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 5, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 2.5, 'MARK_DOWN': 8, 'MARK_UP': 4}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 5, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.5, 'MARK_DOWN': 6, 'MARK_UP': 4}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 5, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.5, 'MARK_DOWN': 6, 'MARK_UP': 6}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 5, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.5, 'MARK_DOWN': 6, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 5, 'CLOSE_WINDOWS': 10, 'QUICK_LENGTH': 7, 'SLOW_LENGTH': 50, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0, 'MARK_DOWN': 8, 'MARK_UP': 4}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 5, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 2.5, 'MARK_DOWN': 8, 'MARK_UP': 4}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 10, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 7, 'SLOW_LENGTH': 40, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.5, 'MARK_DOWN': 8, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 5, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0.5, 'MARK_DOWN': 4, 'MARK_UP': 6}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 5, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0.5, 'MARK_DOWN': 4, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.0, 'MARK_DOWN': 4, 'MARK_UP': 4}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 5, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.0, 'MARK_DOWN': 4, 'MARK_UP': 6}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 5, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.0, 'MARK_DOWN': 4, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0, 'MARK_DOWN': 6, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 7, 'OPEN_RATIO': 2.0, 'MARK_DOWN': 4, 'MARK_UP': 4}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 10, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 7, 'OPEN_RATIO': 2.0, 'MARK_DOWN': 4, 'MARK_UP': 6}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 7, 'OPEN_RATIO': 2.5, 'MARK_DOWN': 6, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0.5, 'MARK_DOWN': 4, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 5, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 2.5, 'MARK_DOWN': 6, 'MARK_UP': 4}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 10, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 7, 'OPEN_RATIO': 2.5, 'MARK_DOWN': 6, 'MARK_UP': 4}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 10, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 7, 'OPEN_RATIO': 2.5, 'MARK_DOWN': 6, 'MARK_UP': 6}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 10, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0.5, 'MARK_DOWN': 4, 'MARK_UP': 4}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 10, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0, 'MARK_DOWN': 4, 'MARK_UP': 4}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 10, 'CLOSE_WINDOWS': 5, 'QUICK_LENGTH': 7, 'SLOW_LENGTH': 40, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.5, 'MARK_DOWN': 4, 'MARK_UP': 4}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 10, 'CLOSE_WINDOWS': 5, 'QUICK_LENGTH': 7, 'SLOW_LENGTH': 40, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.5, 'MARK_DOWN': 4, 'MARK_UP': 6}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 10, 'CLOSE_WINDOWS': 5, 'QUICK_LENGTH': 7, 'SLOW_LENGTH': 40, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.5, 'MARK_DOWN': 4, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 10, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 7, 'OPEN_RATIO': 2.5, 'MARK_DOWN': 8, 'MARK_UP': 4}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 10, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 7, 'OPEN_RATIO': 2.5, 'MARK_DOWN': 8, 'MARK_UP': 6}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 10, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 7, 'OPEN_RATIO': 2.5, 'MARK_DOWN': 8, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0.5, 'MARK_DOWN': 6, 'MARK_UP': 6}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 10, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 2.0, 'MARK_DOWN': 4, 'MARK_UP': 6}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 10, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 2.0, 'MARK_DOWN': 4, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 10, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 5, 'OPEN_RATIO': 2.0, 'MARK_DOWN': 4, 'MARK_UP': 4}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 50, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.0, 'MARK_DOWN': 8, 'MARK_UP': 6}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 50, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.0, 'MARK_DOWN': 8, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 7, 'OPEN_RATIO': 2.5, 'MARK_DOWN': 8, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 2.5, 'MARK_DOWN': 4, 'MARK_UP': 6}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 2.5, 'MARK_DOWN': 4, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0, 'MARK_DOWN': 6, 'MARK_UP': 6}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 7, 'OPEN_RATIO': 2.5, 'MARK_DOWN': 8, 'MARK_UP': 4}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 7, 'OPEN_RATIO': 2.5, 'MARK_DOWN': 8, 'MARK_UP': 6}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 5, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0.5, 'MARK_DOWN': 4, 'MARK_UP': 4}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 50, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0, 'MARK_DOWN': 6, 'MARK_UP': 4}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 50, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0, 'MARK_DOWN': 4, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0.5, 'MARK_DOWN': 6, 'MARK_UP': 4}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0.5, 'MARK_DOWN': 4, 'MARK_UP': 6}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.5, 'MARK_DOWN': 4, 'MARK_UP': 6}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 5, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.5, 'MARK_DOWN': 4, 'MARK_UP': 6}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 5, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.5, 'MARK_DOWN': 4, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 5, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0, 'MARK_DOWN': 4, 'MARK_UP': 6}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 5, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0, 'MARK_DOWN': 4, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.0, 'MARK_DOWN': 6, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 10, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0, 'MARK_DOWN': 6, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0, 'MARK_DOWN': 4, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 5, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 2.5, 'MARK_DOWN': 8, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 50, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.0, 'MARK_DOWN': 4, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0, 'MARK_DOWN': 6, 'MARK_UP': 4}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.5, 'MARK_DOWN': 4, 'MARK_UP': 4}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 5, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 2.5, 'MARK_DOWN': 8, 'MARK_UP': 6}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 10, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0.5, 'MARK_DOWN': 4, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 50, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.0, 'MARK_DOWN': 6, 'MARK_UP': 6}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 7, 'OPEN_RATIO': 2.5, 'MARK_DOWN': 6, 'MARK_UP': 4}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 10, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.0, 'MARK_DOWN': 6, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 5, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 50, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0, 'MARK_DOWN': 8, 'MARK_UP': 4}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 5, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 50, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0, 'MARK_DOWN': 8, 'MARK_UP': 6}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 5, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 50, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0, 'MARK_DOWN': 8, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 50, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0, 'MARK_DOWN': 6, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 10, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.5, 'MARK_DOWN': 4, 'MARK_UP': 6}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 5, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.5, 'MARK_DOWN': 8, 'MARK_UP': 4}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 5, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.5, 'MARK_DOWN': 8, 'MARK_UP': 6}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 5, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.5, 'MARK_DOWN': 8, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 10, 'CLOSE_WINDOWS': 10, 'QUICK_LENGTH': 7, 'SLOW_LENGTH': 40, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.5, 'MARK_DOWN': 4, 'MARK_UP': 4}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 5, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 7, 'OPEN_RATIO': 2.0, 'MARK_DOWN': 6, 'MARK_UP': 4}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 5, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 7, 'OPEN_RATIO': 2.0, 'MARK_DOWN': 6, 'MARK_UP': 6}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 5, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 7, 'OPEN_RATIO': 2.0, 'MARK_DOWN': 6, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 50, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0, 'MARK_DOWN': 4, 'MARK_UP': 4}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 10, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 7, 'OPEN_RATIO': 2.5, 'MARK_DOWN': 4, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 50, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0.5, 'MARK_DOWN': 8, 'MARK_UP': 6}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 50, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0.5, 'MARK_DOWN': 8, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 5, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 7, 'SLOW_LENGTH': 50, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0, 'MARK_DOWN': 8, 'MARK_UP': 4}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 10, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 7, 'SLOW_LENGTH': 40, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.5, 'MARK_DOWN': 6, 'MARK_UP': 4}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 10, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.0, 'MARK_DOWN': 4, 'MARK_UP': 4}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 10, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 7, 'SLOW_LENGTH': 40, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.0, 'MARK_DOWN': 4, 'MARK_UP': 6}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 10, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.0, 'MARK_DOWN': 8, 'MARK_UP': 4}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 10, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.0, 'MARK_DOWN': 8, 'MARK_UP': 6}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 10, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 7, 'OPEN_RATIO': 1.0, 'MARK_DOWN': 8, 'MARK_UP': 8}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 7, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 5, 'OPEN_RATIO': 2.5, 'MARK_DOWN': 4, 'MARK_UP': 6}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 15, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0, 'MARK_DOWN': 4, 'MARK_UP': 6}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 10, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 2.5, 'MARK_DOWN': 8, 'MARK_UP': 4}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 5, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 20, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0, 'MARK_DOWN': 4, 'MARK_UP': 4}</t>
+  </si>
+  <si>
+    <t>{'init_pos': 0, 'init_entry_price': 0, 'fixed_size': 1, 'pricetick': 1, 'HeYueJiaZhi': 100000, 'HeYueChengShu': 10.0, 'Kxian': 15, 'CLOSE_WINDOWS': 10, 'QUICK_LENGTH': 3, 'SLOW_LENGTH': 30, 'CUT_LENGTH': 7, 'OPEN_RATIO': 0.5, 'MARK_DOWN': 6, 'MARK_UP': 4}</t>
   </si>
 </sst>
 </file>
@@ -751,10 +1249,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C104"/>
+  <dimension ref="A1:C270"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A105" sqref="A105:XFD199"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection sqref="A1:C270"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -792,7 +1290,7 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -803,7 +1301,7 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -814,7 +1312,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -825,7 +1323,7 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -836,7 +1334,7 @@
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -847,7 +1345,7 @@
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -858,7 +1356,7 @@
         <v>4</v>
       </c>
       <c r="C9" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -869,7 +1367,7 @@
         <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -880,7 +1378,7 @@
         <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -891,7 +1389,7 @@
         <v>4</v>
       </c>
       <c r="C12" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -902,7 +1400,7 @@
         <v>4</v>
       </c>
       <c r="C13" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -913,7 +1411,7 @@
         <v>4</v>
       </c>
       <c r="C14" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -924,7 +1422,7 @@
         <v>4</v>
       </c>
       <c r="C15" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -935,7 +1433,7 @@
         <v>4</v>
       </c>
       <c r="C16" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -946,7 +1444,7 @@
         <v>4</v>
       </c>
       <c r="C17" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -957,7 +1455,7 @@
         <v>4</v>
       </c>
       <c r="C18" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -968,7 +1466,7 @@
         <v>4</v>
       </c>
       <c r="C19" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -979,7 +1477,7 @@
         <v>4</v>
       </c>
       <c r="C20" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -990,7 +1488,7 @@
         <v>4</v>
       </c>
       <c r="C21" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -1001,7 +1499,7 @@
         <v>4</v>
       </c>
       <c r="C22" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -1012,7 +1510,7 @@
         <v>4</v>
       </c>
       <c r="C23" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -1023,7 +1521,7 @@
         <v>4</v>
       </c>
       <c r="C24" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -1034,7 +1532,7 @@
         <v>4</v>
       </c>
       <c r="C25" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -1045,7 +1543,7 @@
         <v>4</v>
       </c>
       <c r="C26" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -1056,7 +1554,7 @@
         <v>4</v>
       </c>
       <c r="C27" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -1067,7 +1565,7 @@
         <v>4</v>
       </c>
       <c r="C28" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -1078,7 +1576,7 @@
         <v>4</v>
       </c>
       <c r="C29" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -1089,7 +1587,7 @@
         <v>4</v>
       </c>
       <c r="C30" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -1100,7 +1598,7 @@
         <v>4</v>
       </c>
       <c r="C31" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
@@ -1111,7 +1609,7 @@
         <v>4</v>
       </c>
       <c r="C32" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
@@ -1122,7 +1620,7 @@
         <v>4</v>
       </c>
       <c r="C33" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
@@ -1133,7 +1631,7 @@
         <v>4</v>
       </c>
       <c r="C34" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
@@ -1144,7 +1642,7 @@
         <v>4</v>
       </c>
       <c r="C35" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
@@ -1155,7 +1653,7 @@
         <v>4</v>
       </c>
       <c r="C36" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
@@ -1166,7 +1664,7 @@
         <v>4</v>
       </c>
       <c r="C37" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
@@ -1177,7 +1675,7 @@
         <v>4</v>
       </c>
       <c r="C38" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
@@ -1188,7 +1686,7 @@
         <v>4</v>
       </c>
       <c r="C39" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
@@ -1199,7 +1697,7 @@
         <v>4</v>
       </c>
       <c r="C40" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
@@ -1210,7 +1708,7 @@
         <v>4</v>
       </c>
       <c r="C41" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
@@ -1221,7 +1719,7 @@
         <v>4</v>
       </c>
       <c r="C42" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
@@ -1232,7 +1730,7 @@
         <v>4</v>
       </c>
       <c r="C43" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
@@ -1243,7 +1741,7 @@
         <v>4</v>
       </c>
       <c r="C44" t="s">
-        <v>47</v>
+        <v>13</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
@@ -1254,7 +1752,7 @@
         <v>4</v>
       </c>
       <c r="C45" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
@@ -1265,7 +1763,7 @@
         <v>4</v>
       </c>
       <c r="C46" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
@@ -1276,7 +1774,7 @@
         <v>4</v>
       </c>
       <c r="C47" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
@@ -1287,7 +1785,7 @@
         <v>4</v>
       </c>
       <c r="C48" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
@@ -1298,7 +1796,7 @@
         <v>4</v>
       </c>
       <c r="C49" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
@@ -1309,7 +1807,7 @@
         <v>4</v>
       </c>
       <c r="C50" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
@@ -1320,7 +1818,7 @@
         <v>4</v>
       </c>
       <c r="C51" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
@@ -1331,7 +1829,7 @@
         <v>4</v>
       </c>
       <c r="C52" t="s">
-        <v>55</v>
+        <v>17</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
@@ -1342,7 +1840,7 @@
         <v>4</v>
       </c>
       <c r="C53" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
@@ -1353,7 +1851,7 @@
         <v>4</v>
       </c>
       <c r="C54" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
@@ -1364,7 +1862,7 @@
         <v>4</v>
       </c>
       <c r="C55" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
@@ -1375,7 +1873,7 @@
         <v>4</v>
       </c>
       <c r="C56" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
@@ -1386,7 +1884,7 @@
         <v>4</v>
       </c>
       <c r="C57" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
@@ -1397,7 +1895,7 @@
         <v>4</v>
       </c>
       <c r="C58" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
@@ -1408,7 +1906,7 @@
         <v>4</v>
       </c>
       <c r="C59" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
@@ -1419,7 +1917,7 @@
         <v>4</v>
       </c>
       <c r="C60" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
@@ -1430,7 +1928,7 @@
         <v>4</v>
       </c>
       <c r="C61" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
@@ -1441,7 +1939,7 @@
         <v>4</v>
       </c>
       <c r="C62" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
@@ -1452,7 +1950,7 @@
         <v>4</v>
       </c>
       <c r="C63" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
@@ -1463,7 +1961,7 @@
         <v>4</v>
       </c>
       <c r="C64" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
@@ -1474,7 +1972,7 @@
         <v>4</v>
       </c>
       <c r="C65" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
@@ -1485,7 +1983,7 @@
         <v>4</v>
       </c>
       <c r="C66" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
@@ -1496,7 +1994,7 @@
         <v>4</v>
       </c>
       <c r="C67" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
@@ -1507,7 +2005,7 @@
         <v>4</v>
       </c>
       <c r="C68" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
@@ -1518,7 +2016,7 @@
         <v>4</v>
       </c>
       <c r="C69" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
@@ -1529,7 +2027,7 @@
         <v>4</v>
       </c>
       <c r="C70" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
@@ -1540,7 +2038,7 @@
         <v>4</v>
       </c>
       <c r="C71" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
@@ -1551,7 +2049,7 @@
         <v>4</v>
       </c>
       <c r="C72" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
@@ -1562,7 +2060,7 @@
         <v>4</v>
       </c>
       <c r="C73" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
@@ -1573,7 +2071,7 @@
         <v>4</v>
       </c>
       <c r="C74" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
@@ -1584,7 +2082,7 @@
         <v>4</v>
       </c>
       <c r="C75" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
@@ -1595,7 +2093,7 @@
         <v>4</v>
       </c>
       <c r="C76" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
@@ -1606,7 +2104,7 @@
         <v>4</v>
       </c>
       <c r="C77" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
@@ -1617,7 +2115,7 @@
         <v>4</v>
       </c>
       <c r="C78" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
@@ -1628,7 +2126,7 @@
         <v>4</v>
       </c>
       <c r="C79" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
@@ -1639,7 +2137,7 @@
         <v>4</v>
       </c>
       <c r="C80" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
@@ -1650,7 +2148,7 @@
         <v>4</v>
       </c>
       <c r="C81" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
@@ -1661,7 +2159,7 @@
         <v>4</v>
       </c>
       <c r="C82" t="s">
-        <v>85</v>
+        <v>15</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
@@ -1672,7 +2170,7 @@
         <v>4</v>
       </c>
       <c r="C83" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
@@ -1683,7 +2181,7 @@
         <v>4</v>
       </c>
       <c r="C84" t="s">
-        <v>87</v>
+        <v>21</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
@@ -1694,7 +2192,7 @@
         <v>4</v>
       </c>
       <c r="C85" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
@@ -1705,7 +2203,7 @@
         <v>4</v>
       </c>
       <c r="C86" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
@@ -1716,7 +2214,7 @@
         <v>4</v>
       </c>
       <c r="C87" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
@@ -1727,7 +2225,7 @@
         <v>4</v>
       </c>
       <c r="C88" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
@@ -1738,7 +2236,7 @@
         <v>4</v>
       </c>
       <c r="C89" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
@@ -1749,7 +2247,7 @@
         <v>4</v>
       </c>
       <c r="C90" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
@@ -1760,7 +2258,7 @@
         <v>4</v>
       </c>
       <c r="C91" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
@@ -1771,7 +2269,7 @@
         <v>4</v>
       </c>
       <c r="C92" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
@@ -1782,7 +2280,7 @@
         <v>4</v>
       </c>
       <c r="C93" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
@@ -1793,7 +2291,7 @@
         <v>4</v>
       </c>
       <c r="C94" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
@@ -1804,7 +2302,7 @@
         <v>4</v>
       </c>
       <c r="C95" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
@@ -1815,7 +2313,7 @@
         <v>4</v>
       </c>
       <c r="C96" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
@@ -1826,7 +2324,7 @@
         <v>4</v>
       </c>
       <c r="C97" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
@@ -1837,7 +2335,7 @@
         <v>4</v>
       </c>
       <c r="C98" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
@@ -1848,7 +2346,7 @@
         <v>4</v>
       </c>
       <c r="C99" t="s">
-        <v>102</v>
+        <v>19</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
@@ -1859,7 +2357,7 @@
         <v>4</v>
       </c>
       <c r="C100" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
@@ -1870,7 +2368,7 @@
         <v>4</v>
       </c>
       <c r="C101" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
@@ -1881,7 +2379,7 @@
         <v>4</v>
       </c>
       <c r="C102" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
@@ -1892,7 +2390,7 @@
         <v>4</v>
       </c>
       <c r="C103" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
@@ -1903,7 +2401,1833 @@
         <v>4</v>
       </c>
       <c r="C104" t="s">
-        <v>107</v>
+        <v>111</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>3</v>
+      </c>
+      <c r="B105" t="s">
+        <v>4</v>
+      </c>
+      <c r="C105" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>3</v>
+      </c>
+      <c r="B106" t="s">
+        <v>4</v>
+      </c>
+      <c r="C106" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>3</v>
+      </c>
+      <c r="B107" t="s">
+        <v>4</v>
+      </c>
+      <c r="C107" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>3</v>
+      </c>
+      <c r="B108" t="s">
+        <v>4</v>
+      </c>
+      <c r="C108" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>3</v>
+      </c>
+      <c r="B109" t="s">
+        <v>4</v>
+      </c>
+      <c r="C109" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>3</v>
+      </c>
+      <c r="B110" t="s">
+        <v>4</v>
+      </c>
+      <c r="C110" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>3</v>
+      </c>
+      <c r="B111" t="s">
+        <v>4</v>
+      </c>
+      <c r="C111" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>3</v>
+      </c>
+      <c r="B112" t="s">
+        <v>4</v>
+      </c>
+      <c r="C112" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>3</v>
+      </c>
+      <c r="B113" t="s">
+        <v>4</v>
+      </c>
+      <c r="C113" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>3</v>
+      </c>
+      <c r="B114" t="s">
+        <v>4</v>
+      </c>
+      <c r="C114" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
+        <v>3</v>
+      </c>
+      <c r="B115" t="s">
+        <v>4</v>
+      </c>
+      <c r="C115" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>3</v>
+      </c>
+      <c r="B116" t="s">
+        <v>4</v>
+      </c>
+      <c r="C116" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>3</v>
+      </c>
+      <c r="B117" t="s">
+        <v>4</v>
+      </c>
+      <c r="C117" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>3</v>
+      </c>
+      <c r="B118" t="s">
+        <v>4</v>
+      </c>
+      <c r="C118" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>3</v>
+      </c>
+      <c r="B119" t="s">
+        <v>4</v>
+      </c>
+      <c r="C119" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
+        <v>3</v>
+      </c>
+      <c r="B120" t="s">
+        <v>4</v>
+      </c>
+      <c r="C120" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
+        <v>3</v>
+      </c>
+      <c r="B121" t="s">
+        <v>4</v>
+      </c>
+      <c r="C121" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
+        <v>3</v>
+      </c>
+      <c r="B122" t="s">
+        <v>4</v>
+      </c>
+      <c r="C122" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
+        <v>3</v>
+      </c>
+      <c r="B123" t="s">
+        <v>4</v>
+      </c>
+      <c r="C123" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A124" t="s">
+        <v>3</v>
+      </c>
+      <c r="B124" t="s">
+        <v>4</v>
+      </c>
+      <c r="C124" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
+        <v>3</v>
+      </c>
+      <c r="B125" t="s">
+        <v>4</v>
+      </c>
+      <c r="C125" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
+        <v>3</v>
+      </c>
+      <c r="B126" t="s">
+        <v>4</v>
+      </c>
+      <c r="C126" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
+        <v>3</v>
+      </c>
+      <c r="B127" t="s">
+        <v>4</v>
+      </c>
+      <c r="C127" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
+        <v>3</v>
+      </c>
+      <c r="B128" t="s">
+        <v>4</v>
+      </c>
+      <c r="C128" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
+        <v>3</v>
+      </c>
+      <c r="B129" t="s">
+        <v>4</v>
+      </c>
+      <c r="C129" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
+        <v>3</v>
+      </c>
+      <c r="B130" t="s">
+        <v>4</v>
+      </c>
+      <c r="C130" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
+        <v>3</v>
+      </c>
+      <c r="B131" t="s">
+        <v>4</v>
+      </c>
+      <c r="C131" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
+        <v>3</v>
+      </c>
+      <c r="B132" t="s">
+        <v>4</v>
+      </c>
+      <c r="C132" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
+        <v>3</v>
+      </c>
+      <c r="B133" t="s">
+        <v>4</v>
+      </c>
+      <c r="C133" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
+        <v>3</v>
+      </c>
+      <c r="B134" t="s">
+        <v>4</v>
+      </c>
+      <c r="C134" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
+        <v>3</v>
+      </c>
+      <c r="B135" t="s">
+        <v>4</v>
+      </c>
+      <c r="C135" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A136" t="s">
+        <v>3</v>
+      </c>
+      <c r="B136" t="s">
+        <v>4</v>
+      </c>
+      <c r="C136" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
+        <v>3</v>
+      </c>
+      <c r="B137" t="s">
+        <v>4</v>
+      </c>
+      <c r="C137" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
+        <v>3</v>
+      </c>
+      <c r="B138" t="s">
+        <v>4</v>
+      </c>
+      <c r="C138" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
+        <v>3</v>
+      </c>
+      <c r="B139" t="s">
+        <v>4</v>
+      </c>
+      <c r="C139" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A140" t="s">
+        <v>3</v>
+      </c>
+      <c r="B140" t="s">
+        <v>4</v>
+      </c>
+      <c r="C140" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
+        <v>3</v>
+      </c>
+      <c r="B141" t="s">
+        <v>4</v>
+      </c>
+      <c r="C141" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
+        <v>3</v>
+      </c>
+      <c r="B142" t="s">
+        <v>4</v>
+      </c>
+      <c r="C142" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
+        <v>3</v>
+      </c>
+      <c r="B143" t="s">
+        <v>4</v>
+      </c>
+      <c r="C143" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
+        <v>3</v>
+      </c>
+      <c r="B144" t="s">
+        <v>4</v>
+      </c>
+      <c r="C144" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A145" t="s">
+        <v>3</v>
+      </c>
+      <c r="B145" t="s">
+        <v>4</v>
+      </c>
+      <c r="C145" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A146" t="s">
+        <v>3</v>
+      </c>
+      <c r="B146" t="s">
+        <v>4</v>
+      </c>
+      <c r="C146" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A147" t="s">
+        <v>3</v>
+      </c>
+      <c r="B147" t="s">
+        <v>4</v>
+      </c>
+      <c r="C147" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A148" t="s">
+        <v>3</v>
+      </c>
+      <c r="B148" t="s">
+        <v>4</v>
+      </c>
+      <c r="C148" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A149" t="s">
+        <v>3</v>
+      </c>
+      <c r="B149" t="s">
+        <v>4</v>
+      </c>
+      <c r="C149" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A150" t="s">
+        <v>3</v>
+      </c>
+      <c r="B150" t="s">
+        <v>4</v>
+      </c>
+      <c r="C150" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A151" t="s">
+        <v>3</v>
+      </c>
+      <c r="B151" t="s">
+        <v>4</v>
+      </c>
+      <c r="C151" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A152" t="s">
+        <v>3</v>
+      </c>
+      <c r="B152" t="s">
+        <v>4</v>
+      </c>
+      <c r="C152" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A153" t="s">
+        <v>3</v>
+      </c>
+      <c r="B153" t="s">
+        <v>4</v>
+      </c>
+      <c r="C153" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A154" t="s">
+        <v>3</v>
+      </c>
+      <c r="B154" t="s">
+        <v>4</v>
+      </c>
+      <c r="C154" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A155" t="s">
+        <v>3</v>
+      </c>
+      <c r="B155" t="s">
+        <v>4</v>
+      </c>
+      <c r="C155" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A156" t="s">
+        <v>3</v>
+      </c>
+      <c r="B156" t="s">
+        <v>4</v>
+      </c>
+      <c r="C156" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A157" t="s">
+        <v>3</v>
+      </c>
+      <c r="B157" t="s">
+        <v>4</v>
+      </c>
+      <c r="C157" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A158" t="s">
+        <v>3</v>
+      </c>
+      <c r="B158" t="s">
+        <v>4</v>
+      </c>
+      <c r="C158" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A159" t="s">
+        <v>3</v>
+      </c>
+      <c r="B159" t="s">
+        <v>4</v>
+      </c>
+      <c r="C159" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A160" t="s">
+        <v>3</v>
+      </c>
+      <c r="B160" t="s">
+        <v>4</v>
+      </c>
+      <c r="C160" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A161" t="s">
+        <v>3</v>
+      </c>
+      <c r="B161" t="s">
+        <v>4</v>
+      </c>
+      <c r="C161" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A162" t="s">
+        <v>3</v>
+      </c>
+      <c r="B162" t="s">
+        <v>4</v>
+      </c>
+      <c r="C162" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A163" t="s">
+        <v>3</v>
+      </c>
+      <c r="B163" t="s">
+        <v>4</v>
+      </c>
+      <c r="C163" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A164" t="s">
+        <v>3</v>
+      </c>
+      <c r="B164" t="s">
+        <v>4</v>
+      </c>
+      <c r="C164" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A165" t="s">
+        <v>3</v>
+      </c>
+      <c r="B165" t="s">
+        <v>4</v>
+      </c>
+      <c r="C165" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A166" t="s">
+        <v>3</v>
+      </c>
+      <c r="B166" t="s">
+        <v>4</v>
+      </c>
+      <c r="C166" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A167" t="s">
+        <v>3</v>
+      </c>
+      <c r="B167" t="s">
+        <v>4</v>
+      </c>
+      <c r="C167" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A168" t="s">
+        <v>3</v>
+      </c>
+      <c r="B168" t="s">
+        <v>4</v>
+      </c>
+      <c r="C168" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A169" t="s">
+        <v>3</v>
+      </c>
+      <c r="B169" t="s">
+        <v>4</v>
+      </c>
+      <c r="C169" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A170" t="s">
+        <v>3</v>
+      </c>
+      <c r="B170" t="s">
+        <v>4</v>
+      </c>
+      <c r="C170" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A171" t="s">
+        <v>3</v>
+      </c>
+      <c r="B171" t="s">
+        <v>4</v>
+      </c>
+      <c r="C171" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A172" t="s">
+        <v>3</v>
+      </c>
+      <c r="B172" t="s">
+        <v>4</v>
+      </c>
+      <c r="C172" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A173" t="s">
+        <v>3</v>
+      </c>
+      <c r="B173" t="s">
+        <v>4</v>
+      </c>
+      <c r="C173" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A174" t="s">
+        <v>3</v>
+      </c>
+      <c r="B174" t="s">
+        <v>4</v>
+      </c>
+      <c r="C174" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A175" t="s">
+        <v>3</v>
+      </c>
+      <c r="B175" t="s">
+        <v>4</v>
+      </c>
+      <c r="C175" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A176" t="s">
+        <v>3</v>
+      </c>
+      <c r="B176" t="s">
+        <v>4</v>
+      </c>
+      <c r="C176" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A177" t="s">
+        <v>3</v>
+      </c>
+      <c r="B177" t="s">
+        <v>4</v>
+      </c>
+      <c r="C177" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A178" t="s">
+        <v>3</v>
+      </c>
+      <c r="B178" t="s">
+        <v>4</v>
+      </c>
+      <c r="C178" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A179" t="s">
+        <v>3</v>
+      </c>
+      <c r="B179" t="s">
+        <v>4</v>
+      </c>
+      <c r="C179" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A180" t="s">
+        <v>3</v>
+      </c>
+      <c r="B180" t="s">
+        <v>4</v>
+      </c>
+      <c r="C180" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A181" t="s">
+        <v>3</v>
+      </c>
+      <c r="B181" t="s">
+        <v>4</v>
+      </c>
+      <c r="C181" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A182" t="s">
+        <v>3</v>
+      </c>
+      <c r="B182" t="s">
+        <v>4</v>
+      </c>
+      <c r="C182" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A183" t="s">
+        <v>3</v>
+      </c>
+      <c r="B183" t="s">
+        <v>4</v>
+      </c>
+      <c r="C183" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A184" t="s">
+        <v>3</v>
+      </c>
+      <c r="B184" t="s">
+        <v>4</v>
+      </c>
+      <c r="C184" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A185" t="s">
+        <v>3</v>
+      </c>
+      <c r="B185" t="s">
+        <v>4</v>
+      </c>
+      <c r="C185" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A186" t="s">
+        <v>3</v>
+      </c>
+      <c r="B186" t="s">
+        <v>4</v>
+      </c>
+      <c r="C186" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A187" t="s">
+        <v>3</v>
+      </c>
+      <c r="B187" t="s">
+        <v>4</v>
+      </c>
+      <c r="C187" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A188" t="s">
+        <v>3</v>
+      </c>
+      <c r="B188" t="s">
+        <v>4</v>
+      </c>
+      <c r="C188" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A189" t="s">
+        <v>3</v>
+      </c>
+      <c r="B189" t="s">
+        <v>4</v>
+      </c>
+      <c r="C189" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A190" t="s">
+        <v>3</v>
+      </c>
+      <c r="B190" t="s">
+        <v>4</v>
+      </c>
+      <c r="C190" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A191" t="s">
+        <v>3</v>
+      </c>
+      <c r="B191" t="s">
+        <v>4</v>
+      </c>
+      <c r="C191" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A192" t="s">
+        <v>3</v>
+      </c>
+      <c r="B192" t="s">
+        <v>4</v>
+      </c>
+      <c r="C192" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A193" t="s">
+        <v>3</v>
+      </c>
+      <c r="B193" t="s">
+        <v>4</v>
+      </c>
+      <c r="C193" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A194" t="s">
+        <v>3</v>
+      </c>
+      <c r="B194" t="s">
+        <v>4</v>
+      </c>
+      <c r="C194" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A195" t="s">
+        <v>3</v>
+      </c>
+      <c r="B195" t="s">
+        <v>4</v>
+      </c>
+      <c r="C195" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A196" t="s">
+        <v>3</v>
+      </c>
+      <c r="B196" t="s">
+        <v>4</v>
+      </c>
+      <c r="C196" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A197" t="s">
+        <v>3</v>
+      </c>
+      <c r="B197" t="s">
+        <v>4</v>
+      </c>
+      <c r="C197" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A198" t="s">
+        <v>3</v>
+      </c>
+      <c r="B198" t="s">
+        <v>4</v>
+      </c>
+      <c r="C198" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A199" t="s">
+        <v>3</v>
+      </c>
+      <c r="B199" t="s">
+        <v>4</v>
+      </c>
+      <c r="C199" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A200" t="s">
+        <v>3</v>
+      </c>
+      <c r="B200" t="s">
+        <v>4</v>
+      </c>
+      <c r="C200" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A201" t="s">
+        <v>3</v>
+      </c>
+      <c r="B201" t="s">
+        <v>4</v>
+      </c>
+      <c r="C201" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A202" t="s">
+        <v>3</v>
+      </c>
+      <c r="B202" t="s">
+        <v>4</v>
+      </c>
+      <c r="C202" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A203" t="s">
+        <v>3</v>
+      </c>
+      <c r="B203" t="s">
+        <v>4</v>
+      </c>
+      <c r="C203" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A204" t="s">
+        <v>3</v>
+      </c>
+      <c r="B204" t="s">
+        <v>4</v>
+      </c>
+      <c r="C204" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A205" t="s">
+        <v>3</v>
+      </c>
+      <c r="B205" t="s">
+        <v>4</v>
+      </c>
+      <c r="C205" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A206" t="s">
+        <v>3</v>
+      </c>
+      <c r="B206" t="s">
+        <v>4</v>
+      </c>
+      <c r="C206" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A207" t="s">
+        <v>3</v>
+      </c>
+      <c r="B207" t="s">
+        <v>4</v>
+      </c>
+      <c r="C207" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A208" t="s">
+        <v>3</v>
+      </c>
+      <c r="B208" t="s">
+        <v>4</v>
+      </c>
+      <c r="C208" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A209" t="s">
+        <v>3</v>
+      </c>
+      <c r="B209" t="s">
+        <v>4</v>
+      </c>
+      <c r="C209" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A210" t="s">
+        <v>3</v>
+      </c>
+      <c r="B210" t="s">
+        <v>4</v>
+      </c>
+      <c r="C210" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A211" t="s">
+        <v>3</v>
+      </c>
+      <c r="B211" t="s">
+        <v>4</v>
+      </c>
+      <c r="C211" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A212" t="s">
+        <v>3</v>
+      </c>
+      <c r="B212" t="s">
+        <v>4</v>
+      </c>
+      <c r="C212" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A213" t="s">
+        <v>3</v>
+      </c>
+      <c r="B213" t="s">
+        <v>4</v>
+      </c>
+      <c r="C213" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A214" t="s">
+        <v>3</v>
+      </c>
+      <c r="B214" t="s">
+        <v>4</v>
+      </c>
+      <c r="C214" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A215" t="s">
+        <v>3</v>
+      </c>
+      <c r="B215" t="s">
+        <v>4</v>
+      </c>
+      <c r="C215" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A216" t="s">
+        <v>3</v>
+      </c>
+      <c r="B216" t="s">
+        <v>4</v>
+      </c>
+      <c r="C216" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A217" t="s">
+        <v>3</v>
+      </c>
+      <c r="B217" t="s">
+        <v>4</v>
+      </c>
+      <c r="C217" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A218" t="s">
+        <v>3</v>
+      </c>
+      <c r="B218" t="s">
+        <v>4</v>
+      </c>
+      <c r="C218" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A219" t="s">
+        <v>3</v>
+      </c>
+      <c r="B219" t="s">
+        <v>4</v>
+      </c>
+      <c r="C219" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A220" t="s">
+        <v>3</v>
+      </c>
+      <c r="B220" t="s">
+        <v>4</v>
+      </c>
+      <c r="C220" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A221" t="s">
+        <v>3</v>
+      </c>
+      <c r="B221" t="s">
+        <v>4</v>
+      </c>
+      <c r="C221" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A222" t="s">
+        <v>3</v>
+      </c>
+      <c r="B222" t="s">
+        <v>4</v>
+      </c>
+      <c r="C222" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A223" t="s">
+        <v>3</v>
+      </c>
+      <c r="B223" t="s">
+        <v>4</v>
+      </c>
+      <c r="C223" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A224" t="s">
+        <v>3</v>
+      </c>
+      <c r="B224" t="s">
+        <v>4</v>
+      </c>
+      <c r="C224" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A225" t="s">
+        <v>3</v>
+      </c>
+      <c r="B225" t="s">
+        <v>4</v>
+      </c>
+      <c r="C225" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A226" t="s">
+        <v>3</v>
+      </c>
+      <c r="B226" t="s">
+        <v>4</v>
+      </c>
+      <c r="C226" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A227" t="s">
+        <v>3</v>
+      </c>
+      <c r="B227" t="s">
+        <v>4</v>
+      </c>
+      <c r="C227" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A228" t="s">
+        <v>3</v>
+      </c>
+      <c r="B228" t="s">
+        <v>4</v>
+      </c>
+      <c r="C228" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A229" t="s">
+        <v>3</v>
+      </c>
+      <c r="B229" t="s">
+        <v>4</v>
+      </c>
+      <c r="C229" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="230" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A230" t="s">
+        <v>3</v>
+      </c>
+      <c r="B230" t="s">
+        <v>4</v>
+      </c>
+      <c r="C230" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A231" t="s">
+        <v>3</v>
+      </c>
+      <c r="B231" t="s">
+        <v>4</v>
+      </c>
+      <c r="C231" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A232" t="s">
+        <v>3</v>
+      </c>
+      <c r="B232" t="s">
+        <v>4</v>
+      </c>
+      <c r="C232" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="233" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A233" t="s">
+        <v>3</v>
+      </c>
+      <c r="B233" t="s">
+        <v>4</v>
+      </c>
+      <c r="C233" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A234" t="s">
+        <v>3</v>
+      </c>
+      <c r="B234" t="s">
+        <v>4</v>
+      </c>
+      <c r="C234" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="235" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A235" t="s">
+        <v>3</v>
+      </c>
+      <c r="B235" t="s">
+        <v>4</v>
+      </c>
+      <c r="C235" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A236" t="s">
+        <v>3</v>
+      </c>
+      <c r="B236" t="s">
+        <v>4</v>
+      </c>
+      <c r="C236" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="237" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A237" t="s">
+        <v>3</v>
+      </c>
+      <c r="B237" t="s">
+        <v>4</v>
+      </c>
+      <c r="C237" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A238" t="s">
+        <v>3</v>
+      </c>
+      <c r="B238" t="s">
+        <v>4</v>
+      </c>
+      <c r="C238" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="239" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A239" t="s">
+        <v>3</v>
+      </c>
+      <c r="B239" t="s">
+        <v>4</v>
+      </c>
+      <c r="C239" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="240" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A240" t="s">
+        <v>3</v>
+      </c>
+      <c r="B240" t="s">
+        <v>4</v>
+      </c>
+      <c r="C240" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="241" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A241" t="s">
+        <v>3</v>
+      </c>
+      <c r="B241" t="s">
+        <v>4</v>
+      </c>
+      <c r="C241" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A242" t="s">
+        <v>3</v>
+      </c>
+      <c r="B242" t="s">
+        <v>4</v>
+      </c>
+      <c r="C242" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A243" t="s">
+        <v>3</v>
+      </c>
+      <c r="B243" t="s">
+        <v>4</v>
+      </c>
+      <c r="C243" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="244" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A244" t="s">
+        <v>3</v>
+      </c>
+      <c r="B244" t="s">
+        <v>4</v>
+      </c>
+      <c r="C244" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="245" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A245" t="s">
+        <v>3</v>
+      </c>
+      <c r="B245" t="s">
+        <v>4</v>
+      </c>
+      <c r="C245" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="246" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A246" t="s">
+        <v>3</v>
+      </c>
+      <c r="B246" t="s">
+        <v>4</v>
+      </c>
+      <c r="C246" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="247" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A247" t="s">
+        <v>3</v>
+      </c>
+      <c r="B247" t="s">
+        <v>4</v>
+      </c>
+      <c r="C247" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="248" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A248" t="s">
+        <v>3</v>
+      </c>
+      <c r="B248" t="s">
+        <v>4</v>
+      </c>
+      <c r="C248" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="249" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A249" t="s">
+        <v>3</v>
+      </c>
+      <c r="B249" t="s">
+        <v>4</v>
+      </c>
+      <c r="C249" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="250" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A250" t="s">
+        <v>3</v>
+      </c>
+      <c r="B250" t="s">
+        <v>4</v>
+      </c>
+      <c r="C250" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="251" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A251" t="s">
+        <v>3</v>
+      </c>
+      <c r="B251" t="s">
+        <v>4</v>
+      </c>
+      <c r="C251" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="252" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A252" t="s">
+        <v>3</v>
+      </c>
+      <c r="B252" t="s">
+        <v>4</v>
+      </c>
+      <c r="C252" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="253" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A253" t="s">
+        <v>3</v>
+      </c>
+      <c r="B253" t="s">
+        <v>4</v>
+      </c>
+      <c r="C253" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A254" t="s">
+        <v>3</v>
+      </c>
+      <c r="B254" t="s">
+        <v>4</v>
+      </c>
+      <c r="C254" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="255" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A255" t="s">
+        <v>3</v>
+      </c>
+      <c r="B255" t="s">
+        <v>4</v>
+      </c>
+      <c r="C255" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="256" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A256" t="s">
+        <v>3</v>
+      </c>
+      <c r="B256" t="s">
+        <v>4</v>
+      </c>
+      <c r="C256" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="257" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A257" t="s">
+        <v>3</v>
+      </c>
+      <c r="B257" t="s">
+        <v>4</v>
+      </c>
+      <c r="C257" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="258" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A258" t="s">
+        <v>3</v>
+      </c>
+      <c r="B258" t="s">
+        <v>4</v>
+      </c>
+      <c r="C258" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="259" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A259" t="s">
+        <v>3</v>
+      </c>
+      <c r="B259" t="s">
+        <v>4</v>
+      </c>
+      <c r="C259" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="260" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A260" t="s">
+        <v>3</v>
+      </c>
+      <c r="B260" t="s">
+        <v>4</v>
+      </c>
+      <c r="C260" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="261" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A261" t="s">
+        <v>3</v>
+      </c>
+      <c r="B261" t="s">
+        <v>4</v>
+      </c>
+      <c r="C261" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="262" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A262" t="s">
+        <v>3</v>
+      </c>
+      <c r="B262" t="s">
+        <v>4</v>
+      </c>
+      <c r="C262" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="263" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A263" t="s">
+        <v>3</v>
+      </c>
+      <c r="B263" t="s">
+        <v>4</v>
+      </c>
+      <c r="C263" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="264" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A264" t="s">
+        <v>3</v>
+      </c>
+      <c r="B264" t="s">
+        <v>4</v>
+      </c>
+      <c r="C264" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="265" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A265" t="s">
+        <v>3</v>
+      </c>
+      <c r="B265" t="s">
+        <v>4</v>
+      </c>
+      <c r="C265" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="266" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A266" t="s">
+        <v>3</v>
+      </c>
+      <c r="B266" t="s">
+        <v>4</v>
+      </c>
+      <c r="C266" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="267" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A267" t="s">
+        <v>3</v>
+      </c>
+      <c r="B267" t="s">
+        <v>4</v>
+      </c>
+      <c r="C267" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="268" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A268" t="s">
+        <v>3</v>
+      </c>
+      <c r="B268" t="s">
+        <v>4</v>
+      </c>
+      <c r="C268" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="269" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A269" t="s">
+        <v>3</v>
+      </c>
+      <c r="B269" t="s">
+        <v>4</v>
+      </c>
+      <c r="C269" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="270" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A270" t="s">
+        <v>3</v>
+      </c>
+      <c r="B270" t="s">
+        <v>4</v>
+      </c>
+      <c r="C270" t="s">
+        <v>273</v>
       </c>
     </row>
   </sheetData>

</xml_diff>